<commit_message>
Removing future gitignore trouble files
</commit_message>
<xml_diff>
--- a/src/Records.xlsx
+++ b/src/Records.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G478"/>
+  <dimension ref="A1:G490"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7557,6 +7557,190 @@
         </is>
       </c>
     </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Project : </t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>template</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Created : </t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>2021-05-03</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>22:35:36.386017</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>EMAIL_ID</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>CERTIFICATE_CREATED</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>MAIL_SENT</t>
+        </is>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>participant_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>nlbyqzbqigcs,qvaace@kiabws.com</t>
+        </is>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>nlbyqz,bqigcsqvaace@kiabws.com</t>
+        </is>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>nlbyqzb,qigcsq,vaace@kiabws.com</t>
+        </is>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="F488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+      <c r="G488" t="inlineStr">
+        <is>
+          <t>_</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>